<commit_message>
Pretty good version this yes!
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cicero-my.sharepoint.com/personal/froder_cicero_oslo_no/Documents/Documents/GItRepos/VIMPACT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{046578F4-0D98-47DB-AF01-E8F133D72F63}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{054FA913-6279-4317-87F7-96FDFDA6F4AC}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="23055" yWindow="5700" windowWidth="14400" windowHeight="8250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22440" yWindow="5250" windowWidth="21240" windowHeight="12255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="90">
   <si>
     <t>Account Name</t>
   </si>
@@ -274,6 +274,27 @@
   </si>
   <si>
     <t>30924</t>
+  </si>
+  <si>
+    <t>Interne avdelingsseminar</t>
+  </si>
+  <si>
+    <t>Møtekostnader utlandet</t>
+  </si>
+  <si>
+    <t>Div interne prosjektkostnader</t>
+  </si>
+  <si>
+    <t>Prosjektkostnader Towards2040</t>
+  </si>
+  <si>
+    <t>Medieovervåkning / presseklipp</t>
+  </si>
+  <si>
+    <t>Markering - arrangementer</t>
+  </si>
+  <si>
+    <t>31279</t>
   </si>
 </sst>
 </file>
@@ -349,10 +370,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{519AC8EC-EFA4-4BDF-B9A2-2E3EA7AB5EB4}" name="Table1" displayName="Table1" ref="A1:C61" totalsRowShown="0">
-  <autoFilter ref="A1:C61" xr:uid="{519AC8EC-EFA4-4BDF-B9A2-2E3EA7AB5EB4}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C61">
-    <sortCondition ref="A1:A61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{519AC8EC-EFA4-4BDF-B9A2-2E3EA7AB5EB4}" name="Table1" displayName="Table1" ref="A1:C67" totalsRowShown="0">
+  <autoFilter ref="A1:C67" xr:uid="{519AC8EC-EFA4-4BDF-B9A2-2E3EA7AB5EB4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C65">
+    <sortCondition ref="A1:A65"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{6C020BE4-B13D-4BCB-8B99-63EC07501074}" name="Account"/>
@@ -364,8 +385,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1D9BD224-C968-4EBC-9BC1-6C5FA05E6C4C}" name="Table2" displayName="Table2" ref="E1:F17" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="E1:F17" xr:uid="{1D9BD224-C968-4EBC-9BC1-6C5FA05E6C4C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1D9BD224-C968-4EBC-9BC1-6C5FA05E6C4C}" name="Table2" displayName="Table2" ref="E1:F19" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="E1:F19" xr:uid="{1D9BD224-C968-4EBC-9BC1-6C5FA05E6C4C}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A20D6D89-E9E0-4E5C-AE1E-E3BB08D9A80D}" name="Projects" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{EF414676-9FC6-456C-8B68-F8F69ECEE2DA}" name="Spec4" dataDxfId="0"/>
@@ -637,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,6 +973,12 @@
       <c r="C18">
         <v>99</v>
       </c>
+      <c r="E18" s="1">
+        <v>31316</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -963,6 +990,12 @@
       <c r="C19">
         <v>80</v>
       </c>
+      <c r="E19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -1395,10 +1428,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>7701</v>
+        <v>7700</v>
       </c>
       <c r="B59" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="C59">
         <v>99</v>
@@ -1406,10 +1439,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>7704</v>
+        <v>7701</v>
       </c>
       <c r="B60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C60">
         <v>99</v>
@@ -1417,12 +1450,78 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
+        <v>7702</v>
+      </c>
+      <c r="B61" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>7703</v>
+      </c>
+      <c r="B62" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>7704</v>
+      </c>
+      <c r="B63" t="s">
+        <v>57</v>
+      </c>
+      <c r="C63">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>7710</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B64" t="s">
         <v>58</v>
       </c>
-      <c r="C61">
+      <c r="C64">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>7713</v>
+      </c>
+      <c r="B65" t="s">
+        <v>86</v>
+      </c>
+      <c r="C65">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>7730</v>
+      </c>
+      <c r="B66" t="s">
+        <v>87</v>
+      </c>
+      <c r="C66">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>7320</v>
+      </c>
+      <c r="B67" t="s">
+        <v>88</v>
+      </c>
+      <c r="C67">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"First" commit to GitHub repo
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cicero-my.sharepoint.com/personal/froder_cicero_oslo_no/Documents/Documents/GItRepos/VIMPACT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43322F6D-2E5C-4316-9B61-3E5FB5907D15}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4376346B-D390-46B3-8F9A-C08BFDFC0FEE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,171 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
-  <si>
-    <t>Account Name</t>
-  </si>
-  <si>
-    <t>Reiseregninger - hjelpekonto</t>
-  </si>
-  <si>
-    <t>Utlegg - hjelpekonto</t>
-  </si>
-  <si>
-    <t>Prosjektfinansiert - Publisering</t>
-  </si>
-  <si>
-    <t>Gjesteforsker</t>
-  </si>
-  <si>
-    <t>Gjesteforsker - husleie</t>
-  </si>
-  <si>
-    <t>Gjesteforsker - reise</t>
-  </si>
-  <si>
-    <t>Trekkpliktig diettgodtgjørelse</t>
-  </si>
-  <si>
-    <t>Trekkpliktig nattillegg</t>
-  </si>
-  <si>
-    <t>Komp.tillegg utl trekkpliktig</t>
-  </si>
-  <si>
-    <t>Flyttekostnader, ikke oppg.pl. - IKKE I BRUK</t>
-  </si>
-  <si>
-    <t>Gaver til ansatte</t>
-  </si>
-  <si>
-    <t>Kantine</t>
-  </si>
-  <si>
-    <t>Kantine - div varer og arrangement - IKKE I BRUK</t>
-  </si>
-  <si>
-    <t>HMS - helse/miljø/sikkerhet</t>
-  </si>
-  <si>
-    <t>Treningsstudio</t>
-  </si>
-  <si>
-    <t>HVK/CISsos - felleskapsfremmede tiltak</t>
-  </si>
-  <si>
-    <t>Faglig-sosiale arrangement</t>
-  </si>
-  <si>
-    <t>Inventar</t>
-  </si>
-  <si>
-    <t>IT- mobiltelefoner</t>
-  </si>
-  <si>
-    <t>Utstyr/rekvisita</t>
-  </si>
-  <si>
-    <t>IT- hardware nyinnkjøp</t>
-  </si>
-  <si>
-    <t>IT- software nyinnkjøp</t>
-  </si>
-  <si>
-    <t>IT - diverse</t>
-  </si>
-  <si>
-    <t>IT- andre kostnader</t>
-  </si>
-  <si>
-    <t>Diverse konsulentbistand</t>
-  </si>
-  <si>
-    <t>Abonnement</t>
-  </si>
-  <si>
-    <t>IT- mobiltelefoni (abonement)</t>
-  </si>
-  <si>
-    <t>IT- egenandel mobiltelefoner</t>
-  </si>
-  <si>
-    <t>IT- mobiltelefoni ansatte utekontor</t>
-  </si>
-  <si>
-    <t>Bilgodtgjørelse oppg.pl</t>
-  </si>
-  <si>
-    <t>Bilgodtgjørelse oppg.pl skattepliktig</t>
-  </si>
-  <si>
-    <t>Bilgodtgjørelse passasjertillegg</t>
-  </si>
-  <si>
-    <t>Bilgodtgjørelse tilhengertillegg</t>
-  </si>
-  <si>
-    <t>Reisekostnader ikke oppg.pl. I</t>
-  </si>
-  <si>
-    <t>Diettgodtgjørelse m/overn. hotell</t>
-  </si>
-  <si>
-    <t>Diettgodtgjørelse privat innlosjering</t>
-  </si>
-  <si>
-    <t>Diettgodtgjørelse hybel/brakke</t>
-  </si>
-  <si>
-    <t>Diettgodtgjørelse pensjonat</t>
-  </si>
-  <si>
-    <t>Diettgodtgjørelse u/overn.</t>
-  </si>
-  <si>
-    <t>Nattillegg</t>
-  </si>
-  <si>
-    <t>Publiseringskostnader</t>
-  </si>
-  <si>
-    <t>Representasjon</t>
-  </si>
-  <si>
-    <t>Gaver ikke fradragsberettiget</t>
-  </si>
-  <si>
-    <t>Møtekostander</t>
-  </si>
-  <si>
-    <t>Konferanser deltakelse</t>
-  </si>
-  <si>
-    <t>Styrekostnader</t>
-  </si>
-  <si>
-    <t>Kompetanseheving</t>
-  </si>
-  <si>
-    <t>Stipend trekkpliktig</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Account</t>
   </si>
   <si>
     <t>Task</t>
-  </si>
-  <si>
-    <t>Interne avdelingsseminar</t>
-  </si>
-  <si>
-    <t>Medieovervåkning / presseklipp</t>
-  </si>
-  <si>
-    <t>Markering - arrangementer</t>
-  </si>
-  <si>
-    <t>Kontorrekvisita</t>
   </si>
   <si>
     <t>Towards</t>
@@ -387,14 +228,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{519AC8EC-EFA4-4BDF-B9A2-2E3EA7AB5EB4}" name="Table1" displayName="Table1" ref="A1:C53" totalsRowShown="0">
-  <autoFilter ref="A1:C53" xr:uid="{519AC8EC-EFA4-4BDF-B9A2-2E3EA7AB5EB4}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{519AC8EC-EFA4-4BDF-B9A2-2E3EA7AB5EB4}" name="Table1" displayName="Table1" ref="A1:B53" totalsRowShown="0">
+  <autoFilter ref="A1:B53" xr:uid="{519AC8EC-EFA4-4BDF-B9A2-2E3EA7AB5EB4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B53">
     <sortCondition ref="A1:A53"/>
   </sortState>
-  <tableColumns count="3">
+  <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{6C020BE4-B13D-4BCB-8B99-63EC07501074}" name="Account"/>
-    <tableColumn id="2" xr3:uid="{5208B63D-F2C5-4D23-AD38-E9F262A8E987}" name="Account Name"/>
     <tableColumn id="3" xr3:uid="{F7DE8756-2995-4F0D-8FAD-BC14404CED48}" name="Task"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -402,8 +242,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1D9BD224-C968-4EBC-9BC1-6C5FA05E6C4C}" name="Table2" displayName="Table2" ref="E1:E16" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="E1:E16" xr:uid="{1D9BD224-C968-4EBC-9BC1-6C5FA05E6C4C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1D9BD224-C968-4EBC-9BC1-6C5FA05E6C4C}" name="Table2" displayName="Table2" ref="D1:D16" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="D1:D16" xr:uid="{1D9BD224-C968-4EBC-9BC1-6C5FA05E6C4C}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{A20D6D89-E9E0-4E5C-AE1E-E3BB08D9A80D}" name="Towards" dataDxfId="2"/>
   </tableColumns>
@@ -412,8 +252,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{11C2DD78-57A2-464C-819F-05BC458D5493}" name="Table3" displayName="Table3" ref="G1:G29" totalsRowShown="0" dataDxfId="1">
-  <autoFilter ref="G1:G29" xr:uid="{11C2DD78-57A2-464C-819F-05BC458D5493}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{11C2DD78-57A2-464C-819F-05BC458D5493}" name="Table3" displayName="Table3" ref="F1:F29" totalsRowShown="0" dataDxfId="1">
+  <autoFilter ref="F1:F29" xr:uid="{11C2DD78-57A2-464C-819F-05BC458D5493}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{6C6F5011-27CD-449A-B591-92D65642B659}" name="Project_VAT" dataDxfId="0"/>
   </tableColumns>
@@ -684,736 +524,576 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2931</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>30</v>
-      </c>
-      <c r="E2">
+      <c r="B2">
+        <v>30</v>
+      </c>
+      <c r="D2">
         <v>31441</v>
       </c>
-      <c r="G2" s="5">
+      <c r="F2" s="5">
         <v>30924</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2933</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>80</v>
-      </c>
-      <c r="E3">
+      <c r="B3">
+        <v>80</v>
+      </c>
+      <c r="D3">
         <v>31443</v>
       </c>
-      <c r="G3" s="5">
+      <c r="F3" s="5">
         <v>30949</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4330</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>80</v>
-      </c>
-      <c r="E4">
+      <c r="B4">
+        <v>80</v>
+      </c>
+      <c r="D4">
         <v>31456</v>
       </c>
-      <c r="G4" s="5">
+      <c r="F4" s="5">
         <v>31242</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4530</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5">
+      <c r="B5">
         <v>50</v>
       </c>
-      <c r="E5">
+      <c r="D5">
         <v>31475</v>
       </c>
-      <c r="G5" s="5">
+      <c r="F5" s="5">
         <v>31268</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4532</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6">
+      <c r="B6">
         <v>50</v>
       </c>
-      <c r="E6">
+      <c r="D6">
         <v>31476</v>
       </c>
-      <c r="G6" s="5">
+      <c r="F6" s="5">
         <v>31361</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4534</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
+      <c r="B7">
         <v>51</v>
       </c>
-      <c r="E7">
+      <c r="D7">
         <v>31486</v>
       </c>
-      <c r="G7" s="5">
+      <c r="F7" s="5">
         <v>31379</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5320</v>
       </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>30</v>
-      </c>
-      <c r="E8">
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="D8">
         <v>31487</v>
       </c>
-      <c r="G8" s="5">
+      <c r="F8" s="5">
         <v>31425</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>5321</v>
       </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>30</v>
-      </c>
-      <c r="E9">
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="D9">
         <v>31488</v>
       </c>
-      <c r="G9" s="2">
+      <c r="F9" s="2">
         <v>31445</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>5325</v>
       </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>30</v>
-      </c>
-      <c r="E10">
+      <c r="B10">
+        <v>30</v>
+      </c>
+      <c r="D10">
         <v>31489</v>
       </c>
-      <c r="G10" s="3">
+      <c r="F10" s="3">
         <v>31454</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>5510</v>
       </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>80</v>
-      </c>
-      <c r="E11">
+      <c r="B11">
+        <v>80</v>
+      </c>
+      <c r="D11">
         <v>31490</v>
       </c>
-      <c r="G11" s="2">
+      <c r="F11" s="2">
         <v>31457</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>5555</v>
       </c>
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12">
+      <c r="B12">
         <v>55</v>
       </c>
-      <c r="E12">
+      <c r="D12">
         <v>31499</v>
       </c>
-      <c r="G12" s="3">
+      <c r="F12" s="3">
         <v>31465</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>5900</v>
       </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13">
-        <v>80</v>
-      </c>
-      <c r="E13">
+      <c r="B13">
+        <v>80</v>
+      </c>
+      <c r="D13">
         <v>31511</v>
       </c>
-      <c r="G13" s="2">
+      <c r="F13" s="2">
         <v>31470</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>5910</v>
       </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14">
-        <v>80</v>
-      </c>
-      <c r="E14">
+      <c r="B14">
+        <v>80</v>
+      </c>
+      <c r="D14">
         <v>31512</v>
       </c>
-      <c r="G14" s="3">
+      <c r="F14" s="3">
         <v>31473</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>5912</v>
       </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15">
-        <v>80</v>
-      </c>
-      <c r="E15">
+      <c r="B15">
+        <v>80</v>
+      </c>
+      <c r="D15">
         <v>31520</v>
       </c>
-      <c r="G15" s="2">
+      <c r="F15" s="2">
         <v>31491</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>5950</v>
       </c>
-      <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16">
-        <v>80</v>
-      </c>
-      <c r="E16">
+      <c r="B16">
+        <v>80</v>
+      </c>
+      <c r="D16">
         <v>31316</v>
       </c>
-      <c r="G16" s="3">
+      <c r="F16" s="3">
         <v>31492</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>5960</v>
       </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17">
-        <v>80</v>
-      </c>
-      <c r="G17" s="2">
+      <c r="B17">
+        <v>80</v>
+      </c>
+      <c r="F17" s="2">
         <v>31495</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>5965</v>
       </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18">
+      <c r="B18">
         <v>82</v>
       </c>
-      <c r="G18" s="3">
+      <c r="F18" s="3">
         <v>31503</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>5972</v>
       </c>
-      <c r="B19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19">
+      <c r="B19">
         <v>83</v>
       </c>
-      <c r="G19" s="2">
+      <c r="F19" s="2">
         <v>31504</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>5974</v>
       </c>
-      <c r="B20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20">
-        <v>80</v>
-      </c>
-      <c r="G20" s="3">
+      <c r="B20">
+        <v>80</v>
+      </c>
+      <c r="F20" s="3">
         <v>31505</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>6540</v>
       </c>
-      <c r="B21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21">
-        <v>80</v>
-      </c>
-      <c r="G21" s="2">
+      <c r="B21">
+        <v>80</v>
+      </c>
+      <c r="F21" s="2">
         <v>31507</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>6552</v>
       </c>
-      <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22">
+      <c r="B22">
         <v>81</v>
       </c>
-      <c r="G22" s="3">
+      <c r="F22" s="3">
         <v>31516</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>6560</v>
       </c>
-      <c r="B23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23">
-        <v>80</v>
-      </c>
-      <c r="G23" s="2">
+      <c r="B23">
+        <v>80</v>
+      </c>
+      <c r="F23" s="2">
         <v>31518</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>6580</v>
       </c>
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24">
+      <c r="B24">
         <v>81</v>
       </c>
-      <c r="G24" s="3">
+      <c r="F24" s="3">
         <v>31519</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>6585</v>
       </c>
-      <c r="B25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25">
+      <c r="B25">
         <v>81</v>
       </c>
-      <c r="G25" s="2">
+      <c r="F25" s="2">
         <v>31523</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>6588</v>
       </c>
-      <c r="B26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26">
+      <c r="B26">
         <v>81</v>
       </c>
-      <c r="G26" s="3">
+      <c r="F26" s="3">
         <v>31525</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>6590</v>
       </c>
-      <c r="B27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27">
+      <c r="B27">
         <v>81</v>
       </c>
-      <c r="G27" s="2">
+      <c r="F27" s="2">
         <v>31527</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>6790</v>
       </c>
-      <c r="B28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28">
+      <c r="B28">
         <v>29</v>
       </c>
-      <c r="G28" s="3">
+      <c r="F28" s="3">
         <v>31529</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>6800</v>
       </c>
-      <c r="B29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29">
-        <v>80</v>
-      </c>
-      <c r="G29" s="4">
+      <c r="B29">
+        <v>80</v>
+      </c>
+      <c r="F29" s="4">
         <v>31531</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>6842</v>
       </c>
-      <c r="B30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>6920</v>
       </c>
-      <c r="B31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31">
+      <c r="B31">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>6921</v>
       </c>
-      <c r="B32" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32">
+      <c r="B32">
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>6922</v>
       </c>
-      <c r="B33" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33">
+      <c r="B33">
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>7100</v>
       </c>
-      <c r="B34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>7101</v>
       </c>
-      <c r="B35" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>7102</v>
       </c>
-      <c r="B36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>7103</v>
       </c>
-      <c r="B37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>7140</v>
       </c>
-      <c r="B38" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>7150</v>
       </c>
-      <c r="B39" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>7151</v>
       </c>
-      <c r="B40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>7155</v>
       </c>
-      <c r="B41" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>7156</v>
       </c>
-      <c r="B42" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>7160</v>
       </c>
-      <c r="B43" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>7161</v>
       </c>
-      <c r="B44" t="s">
-        <v>40</v>
-      </c>
-      <c r="C44">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>7305</v>
       </c>
-      <c r="B45" t="s">
-        <v>41</v>
-      </c>
-      <c r="C45">
+      <c r="B45">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>7320</v>
       </c>
-      <c r="B46" t="s">
-        <v>53</v>
-      </c>
-      <c r="C46">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>7350</v>
       </c>
-      <c r="B47" t="s">
-        <v>42</v>
-      </c>
-      <c r="C47">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>7420</v>
       </c>
-      <c r="B48" t="s">
-        <v>43</v>
-      </c>
-      <c r="C48">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>7700</v>
       </c>
-      <c r="B49" t="s">
-        <v>51</v>
-      </c>
-      <c r="C49">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>7701</v>
       </c>
-      <c r="B50" t="s">
-        <v>44</v>
-      </c>
-      <c r="C50">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>7704</v>
       </c>
-      <c r="B51" t="s">
-        <v>45</v>
-      </c>
-      <c r="C51">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>7710</v>
       </c>
-      <c r="B52" t="s">
-        <v>46</v>
-      </c>
-      <c r="C52">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>7730</v>
       </c>
-      <c r="B53" t="s">
-        <v>52</v>
-      </c>
-      <c r="C53">
+      <c r="B53">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed the CICERO-specific accounting mapping.
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cicero-my.sharepoint.com/personal/froder_cicero_oslo_no/Documents/Documents/GItRepos/VIMPACT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4376346B-D390-46B3-8F9A-C08BFDFC0FEE}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42A62264-272B-4309-A89F-4EDE7805C7C1}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3825" yWindow="1785" windowWidth="17325" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -229,7 +229,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{519AC8EC-EFA4-4BDF-B9A2-2E3EA7AB5EB4}" name="Table1" displayName="Table1" ref="A1:B53" totalsRowShown="0">
-  <autoFilter ref="A1:B53" xr:uid="{519AC8EC-EFA4-4BDF-B9A2-2E3EA7AB5EB4}"/>
+  <autoFilter ref="A1:B53" xr:uid="{519AC8EC-EFA4-4BDF-B9A2-2E3EA7AB5EB4}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="81"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B53">
     <sortCondition ref="A1:A53"/>
   </sortState>
@@ -530,15 +536,15 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -552,7 +558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2931</v>
       </c>
@@ -566,7 +572,7 @@
         <v>30924</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2933</v>
       </c>
@@ -580,7 +586,7 @@
         <v>30949</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4330</v>
       </c>
@@ -594,7 +600,7 @@
         <v>31242</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4530</v>
       </c>
@@ -608,7 +614,7 @@
         <v>31268</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4532</v>
       </c>
@@ -622,7 +628,7 @@
         <v>31361</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4534</v>
       </c>
@@ -636,7 +642,7 @@
         <v>31379</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5320</v>
       </c>
@@ -650,7 +656,7 @@
         <v>31425</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5321</v>
       </c>
@@ -664,7 +670,7 @@
         <v>31445</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5325</v>
       </c>
@@ -678,7 +684,7 @@
         <v>31454</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5510</v>
       </c>
@@ -692,7 +698,7 @@
         <v>31457</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5555</v>
       </c>
@@ -706,7 +712,7 @@
         <v>31465</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5900</v>
       </c>
@@ -720,7 +726,7 @@
         <v>31470</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5910</v>
       </c>
@@ -734,7 +740,7 @@
         <v>31473</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5912</v>
       </c>
@@ -748,7 +754,7 @@
         <v>31491</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5950</v>
       </c>
@@ -762,7 +768,7 @@
         <v>31492</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5960</v>
       </c>
@@ -773,7 +779,7 @@
         <v>31495</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5965</v>
       </c>
@@ -784,7 +790,7 @@
         <v>31503</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5972</v>
       </c>
@@ -795,7 +801,7 @@
         <v>31504</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5974</v>
       </c>
@@ -806,7 +812,7 @@
         <v>31505</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6540</v>
       </c>
@@ -817,7 +823,7 @@
         <v>31507</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6552</v>
       </c>
@@ -828,7 +834,7 @@
         <v>31516</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6560</v>
       </c>
@@ -839,7 +845,7 @@
         <v>31518</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6580</v>
       </c>
@@ -850,7 +856,7 @@
         <v>31519</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6585</v>
       </c>
@@ -861,7 +867,7 @@
         <v>31523</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6588</v>
       </c>
@@ -872,7 +878,7 @@
         <v>31525</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>6590</v>
       </c>
@@ -883,7 +889,7 @@
         <v>31527</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6790</v>
       </c>
@@ -894,7 +900,7 @@
         <v>31529</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6800</v>
       </c>
@@ -905,7 +911,7 @@
         <v>31531</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6842</v>
       </c>
@@ -913,7 +919,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6920</v>
       </c>
@@ -921,7 +927,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6921</v>
       </c>
@@ -929,7 +935,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>6922</v>
       </c>
@@ -937,7 +943,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7100</v>
       </c>
@@ -945,7 +951,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7101</v>
       </c>
@@ -953,7 +959,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7102</v>
       </c>
@@ -961,7 +967,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>7103</v>
       </c>
@@ -969,7 +975,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>7140</v>
       </c>
@@ -977,7 +983,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>7150</v>
       </c>
@@ -985,7 +991,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>7151</v>
       </c>
@@ -993,7 +999,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>7155</v>
       </c>
@@ -1001,7 +1007,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>7156</v>
       </c>
@@ -1009,7 +1015,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>7160</v>
       </c>
@@ -1017,7 +1023,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>7161</v>
       </c>
@@ -1025,7 +1031,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>7305</v>
       </c>
@@ -1033,7 +1039,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>7320</v>
       </c>
@@ -1041,7 +1047,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>7350</v>
       </c>
@@ -1049,7 +1055,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>7420</v>
       </c>
@@ -1057,7 +1063,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>7700</v>
       </c>
@@ -1065,7 +1071,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>7701</v>
       </c>
@@ -1073,7 +1079,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>7704</v>
       </c>
@@ -1081,7 +1087,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>7710</v>
       </c>
@@ -1089,7 +1095,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>7730</v>
       </c>

</xml_diff>

<commit_message>
Fixing a row replacemnt bug in cicero_specific_trans.
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cicero-my.sharepoint.com/personal/froder_cicero_oslo_no/Documents/Documents/GItRepos/VIMPACT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42A62264-272B-4309-A89F-4EDE7805C7C1}"/>
+  <xr:revisionPtr revIDLastSave="188" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4D32C85-0C82-4A9F-B5D4-AC33C8A898A4}"/>
   <bookViews>
-    <workbookView xWindow="3825" yWindow="1785" windowWidth="17325" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="8955" yWindow="4710" windowWidth="25335" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -229,13 +229,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{519AC8EC-EFA4-4BDF-B9A2-2E3EA7AB5EB4}" name="Table1" displayName="Table1" ref="A1:B53" totalsRowShown="0">
-  <autoFilter ref="A1:B53" xr:uid="{519AC8EC-EFA4-4BDF-B9A2-2E3EA7AB5EB4}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="81"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:B53" xr:uid="{519AC8EC-EFA4-4BDF-B9A2-2E3EA7AB5EB4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B53">
     <sortCondition ref="A1:A53"/>
   </sortState>
@@ -250,6 +244,9 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1D9BD224-C968-4EBC-9BC1-6C5FA05E6C4C}" name="Table2" displayName="Table2" ref="D1:D16" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="D1:D16" xr:uid="{1D9BD224-C968-4EBC-9BC1-6C5FA05E6C4C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:D16">
+    <sortCondition ref="D1:D16"/>
+  </sortState>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{A20D6D89-E9E0-4E5C-AE1E-E3BB08D9A80D}" name="Towards" dataDxfId="2"/>
   </tableColumns>
@@ -260,6 +257,9 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{11C2DD78-57A2-464C-819F-05BC458D5493}" name="Table3" displayName="Table3" ref="F1:F29" totalsRowShown="0" dataDxfId="1">
   <autoFilter ref="F1:F29" xr:uid="{11C2DD78-57A2-464C-819F-05BC458D5493}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:F29">
+    <sortCondition ref="F1:F29"/>
+  </sortState>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{6C6F5011-27CD-449A-B591-92D65642B659}" name="Project_VAT" dataDxfId="0"/>
   </tableColumns>
@@ -558,7 +558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2931</v>
       </c>
@@ -566,13 +566,13 @@
         <v>30</v>
       </c>
       <c r="D2">
-        <v>31441</v>
+        <v>31316</v>
       </c>
       <c r="F2" s="5">
         <v>30924</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2933</v>
       </c>
@@ -580,13 +580,13 @@
         <v>80</v>
       </c>
       <c r="D3">
-        <v>31443</v>
+        <v>31441</v>
       </c>
       <c r="F3" s="5">
         <v>30949</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4330</v>
       </c>
@@ -594,13 +594,13 @@
         <v>80</v>
       </c>
       <c r="D4">
-        <v>31456</v>
+        <v>31443</v>
       </c>
       <c r="F4" s="5">
         <v>31242</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4530</v>
       </c>
@@ -608,13 +608,13 @@
         <v>50</v>
       </c>
       <c r="D5">
-        <v>31475</v>
+        <v>31456</v>
       </c>
       <c r="F5" s="5">
         <v>31268</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4532</v>
       </c>
@@ -622,13 +622,13 @@
         <v>50</v>
       </c>
       <c r="D6">
-        <v>31476</v>
+        <v>31475</v>
       </c>
       <c r="F6" s="5">
         <v>31361</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4534</v>
       </c>
@@ -636,13 +636,13 @@
         <v>51</v>
       </c>
       <c r="D7">
-        <v>31486</v>
+        <v>31476</v>
       </c>
       <c r="F7" s="5">
         <v>31379</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5320</v>
       </c>
@@ -650,13 +650,13 @@
         <v>30</v>
       </c>
       <c r="D8">
-        <v>31487</v>
+        <v>31486</v>
       </c>
       <c r="F8" s="5">
         <v>31425</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5321</v>
       </c>
@@ -664,13 +664,13 @@
         <v>30</v>
       </c>
       <c r="D9">
-        <v>31488</v>
+        <v>31487</v>
       </c>
       <c r="F9" s="2">
         <v>31445</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5325</v>
       </c>
@@ -678,13 +678,13 @@
         <v>30</v>
       </c>
       <c r="D10">
-        <v>31489</v>
+        <v>31488</v>
       </c>
       <c r="F10" s="3">
         <v>31454</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5510</v>
       </c>
@@ -692,13 +692,13 @@
         <v>80</v>
       </c>
       <c r="D11">
-        <v>31490</v>
+        <v>31489</v>
       </c>
       <c r="F11" s="2">
         <v>31457</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5555</v>
       </c>
@@ -706,13 +706,13 @@
         <v>55</v>
       </c>
       <c r="D12">
-        <v>31499</v>
+        <v>31490</v>
       </c>
       <c r="F12" s="3">
         <v>31465</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5900</v>
       </c>
@@ -720,13 +720,13 @@
         <v>80</v>
       </c>
       <c r="D13">
-        <v>31511</v>
+        <v>31499</v>
       </c>
       <c r="F13" s="2">
         <v>31470</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5910</v>
       </c>
@@ -734,13 +734,13 @@
         <v>80</v>
       </c>
       <c r="D14">
-        <v>31512</v>
+        <v>31511</v>
       </c>
       <c r="F14" s="3">
         <v>31473</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5912</v>
       </c>
@@ -748,13 +748,13 @@
         <v>80</v>
       </c>
       <c r="D15">
-        <v>31520</v>
+        <v>31512</v>
       </c>
       <c r="F15" s="2">
         <v>31491</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5950</v>
       </c>
@@ -762,13 +762,13 @@
         <v>80</v>
       </c>
       <c r="D16">
-        <v>31316</v>
+        <v>31520</v>
       </c>
       <c r="F16" s="3">
         <v>31492</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5960</v>
       </c>
@@ -779,7 +779,7 @@
         <v>31495</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5965</v>
       </c>
@@ -790,7 +790,7 @@
         <v>31503</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5972</v>
       </c>
@@ -801,7 +801,7 @@
         <v>31504</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5974</v>
       </c>
@@ -812,7 +812,7 @@
         <v>31505</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6540</v>
       </c>
@@ -834,7 +834,7 @@
         <v>31516</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6560</v>
       </c>
@@ -889,7 +889,7 @@
         <v>31527</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6790</v>
       </c>
@@ -900,7 +900,7 @@
         <v>31529</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6800</v>
       </c>
@@ -911,7 +911,7 @@
         <v>31531</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6842</v>
       </c>
@@ -943,7 +943,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7100</v>
       </c>
@@ -951,7 +951,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7101</v>
       </c>
@@ -959,7 +959,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7102</v>
       </c>
@@ -967,7 +967,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>7103</v>
       </c>
@@ -975,7 +975,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>7140</v>
       </c>
@@ -983,7 +983,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>7150</v>
       </c>
@@ -991,7 +991,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>7151</v>
       </c>
@@ -999,7 +999,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>7155</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>7156</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>7160</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>7161</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>7305</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>7320</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>7350</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>7420</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>7700</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>7701</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>7704</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>7710</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>7730</v>
       </c>

</xml_diff>

<commit_message>
New version with Maconomy API integration (Azure user auth APIM)
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cicero-my.sharepoint.com/personal/froder_cicero_oslo_no/Documents/Documents/GItRepos/VIMPACT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4D32C85-0C82-4A9F-B5D4-AC33C8A898A4}"/>
+  <xr:revisionPtr revIDLastSave="201" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A503403-FBD8-415E-944F-B6F2D4DD271A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="8955" yWindow="4710" windowWidth="25335" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15630" yWindow="4905" windowWidth="12915" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -81,6 +81,18 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -120,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -129,10 +141,23 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -140,6 +165,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -205,15 +239,6 @@
       </fill>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -242,26 +267,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1D9BD224-C968-4EBC-9BC1-6C5FA05E6C4C}" name="Table2" displayName="Table2" ref="D1:D16" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1D9BD224-C968-4EBC-9BC1-6C5FA05E6C4C}" name="Table2" displayName="Table2" ref="D1:D16" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="D1:D16" xr:uid="{1D9BD224-C968-4EBC-9BC1-6C5FA05E6C4C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:D16">
-    <sortCondition ref="D1:D16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:D15">
+    <sortCondition ref="D1:D15"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A20D6D89-E9E0-4E5C-AE1E-E3BB08D9A80D}" name="Towards" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{A20D6D89-E9E0-4E5C-AE1E-E3BB08D9A80D}" name="Towards" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{11C2DD78-57A2-464C-819F-05BC458D5493}" name="Table3" displayName="Table3" ref="F1:F29" totalsRowShown="0" dataDxfId="1">
-  <autoFilter ref="F1:F29" xr:uid="{11C2DD78-57A2-464C-819F-05BC458D5493}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{11C2DD78-57A2-464C-819F-05BC458D5493}" name="Table3" displayName="Table3" ref="F1:F32" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="F1:F32" xr:uid="{11C2DD78-57A2-464C-819F-05BC458D5493}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:F29">
     <sortCondition ref="F1:F29"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{6C6F5011-27CD-449A-B591-92D65642B659}" name="Project_VAT" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{6C6F5011-27CD-449A-B591-92D65642B659}" name="Project_VAT" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -532,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,9 +591,9 @@
         <v>30</v>
       </c>
       <c r="D2">
-        <v>31316</v>
-      </c>
-      <c r="F2" s="5">
+        <v>31441</v>
+      </c>
+      <c r="F2" s="4">
         <v>30924</v>
       </c>
     </row>
@@ -580,9 +605,9 @@
         <v>80</v>
       </c>
       <c r="D3">
-        <v>31441</v>
-      </c>
-      <c r="F3" s="5">
+        <v>31443</v>
+      </c>
+      <c r="F3" s="4">
         <v>30949</v>
       </c>
     </row>
@@ -594,9 +619,9 @@
         <v>80</v>
       </c>
       <c r="D4">
-        <v>31443</v>
-      </c>
-      <c r="F4" s="5">
+        <v>31456</v>
+      </c>
+      <c r="F4" s="4">
         <v>31242</v>
       </c>
     </row>
@@ -608,9 +633,9 @@
         <v>50</v>
       </c>
       <c r="D5">
-        <v>31456</v>
-      </c>
-      <c r="F5" s="5">
+        <v>31475</v>
+      </c>
+      <c r="F5" s="4">
         <v>31268</v>
       </c>
     </row>
@@ -622,9 +647,9 @@
         <v>50</v>
       </c>
       <c r="D6">
-        <v>31475</v>
-      </c>
-      <c r="F6" s="5">
+        <v>31476</v>
+      </c>
+      <c r="F6" s="6">
         <v>31361</v>
       </c>
     </row>
@@ -636,9 +661,9 @@
         <v>51</v>
       </c>
       <c r="D7">
-        <v>31476</v>
-      </c>
-      <c r="F7" s="5">
+        <v>31486</v>
+      </c>
+      <c r="F7" s="4">
         <v>31379</v>
       </c>
     </row>
@@ -650,9 +675,9 @@
         <v>30</v>
       </c>
       <c r="D8">
-        <v>31486</v>
-      </c>
-      <c r="F8" s="5">
+        <v>31487</v>
+      </c>
+      <c r="F8" s="4">
         <v>31425</v>
       </c>
     </row>
@@ -664,7 +689,7 @@
         <v>30</v>
       </c>
       <c r="D9">
-        <v>31487</v>
+        <v>31488</v>
       </c>
       <c r="F9" s="2">
         <v>31445</v>
@@ -678,7 +703,7 @@
         <v>30</v>
       </c>
       <c r="D10">
-        <v>31488</v>
+        <v>31489</v>
       </c>
       <c r="F10" s="3">
         <v>31454</v>
@@ -692,7 +717,7 @@
         <v>80</v>
       </c>
       <c r="D11">
-        <v>31489</v>
+        <v>31490</v>
       </c>
       <c r="F11" s="2">
         <v>31457</v>
@@ -706,9 +731,9 @@
         <v>55</v>
       </c>
       <c r="D12">
-        <v>31490</v>
-      </c>
-      <c r="F12" s="3">
+        <v>31499</v>
+      </c>
+      <c r="F12" s="7">
         <v>31465</v>
       </c>
     </row>
@@ -720,7 +745,7 @@
         <v>80</v>
       </c>
       <c r="D13">
-        <v>31499</v>
+        <v>31511</v>
       </c>
       <c r="F13" s="2">
         <v>31470</v>
@@ -734,7 +759,7 @@
         <v>80</v>
       </c>
       <c r="D14">
-        <v>31511</v>
+        <v>31512</v>
       </c>
       <c r="F14" s="3">
         <v>31473</v>
@@ -748,7 +773,7 @@
         <v>80</v>
       </c>
       <c r="D15">
-        <v>31512</v>
+        <v>31520</v>
       </c>
       <c r="F15" s="2">
         <v>31491</v>
@@ -761,10 +786,10 @@
       <c r="B16">
         <v>80</v>
       </c>
-      <c r="D16">
-        <v>31520</v>
-      </c>
-      <c r="F16" s="3">
+      <c r="D16" s="5">
+        <v>31544</v>
+      </c>
+      <c r="F16" s="7">
         <v>31492</v>
       </c>
     </row>
@@ -786,7 +811,7 @@
       <c r="B18">
         <v>82</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="7">
         <v>31503</v>
       </c>
     </row>
@@ -885,7 +910,7 @@
       <c r="B27">
         <v>81</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="8">
         <v>31527</v>
       </c>
     </row>
@@ -896,7 +921,7 @@
       <c r="B28">
         <v>29</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="8">
         <v>31529</v>
       </c>
     </row>
@@ -907,7 +932,7 @@
       <c r="B29">
         <v>80</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="9">
         <v>31531</v>
       </c>
     </row>
@@ -918,6 +943,9 @@
       <c r="B30">
         <v>80</v>
       </c>
+      <c r="F30" s="10">
+        <v>31540</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -926,6 +954,9 @@
       <c r="B31">
         <v>81</v>
       </c>
+      <c r="F31" s="10">
+        <v>31541</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -933,6 +964,9 @@
       </c>
       <c r="B32">
         <v>81</v>
+      </c>
+      <c r="F32" s="10">
+        <v>31542</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>